<commit_message>
Fixed bugs in data structure and added unit test
</commit_message>
<xml_diff>
--- a/lookupData/objectives-en.xlsx
+++ b/lookupData/objectives-en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\OneDrive\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67132EB1-9B7C-4BE5-AA1D-0232A5892C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C584409-FA6E-4865-98DF-6F061274806D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="637">
   <si>
     <t>In-game description</t>
   </si>
@@ -1993,35 +1993,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="22">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2055,6 +2039,36 @@
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2069,37 +2083,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11298E10-21DD-4EBF-8BF9-EA571BEEC72E}" name="Table1" displayName="Table1" ref="A2:H127" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A2:H127" xr:uid="{11298E10-21DD-4EBF-8BF9-EA571BEEC72E}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{324771F9-822A-49B7-893D-1DA308D60F66}" name="Achievment" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{B22A3C33-D5FF-489D-81A0-0CD56EF167F6}" name="In-game description" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{3735BB57-B1D2-421D-9276-41B28AD37626}" name="Actual requirements (if different)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{F9AD4A86-89AB-4252-BDC8-8698B593B077}" name="#" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{36B12DC4-1FAB-47F0-B495-DEEF3597AFFC}" name="Category" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{8DA34B88-F916-4B29-AA18-6228488B3C65}" name="Object" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{132DC9C0-CA6E-4B12-886A-9AB9F8BB67DB}" name="Index" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{ED2AFE63-C022-4969-A969-B12DDDC6F848}" name="Achievement (English Title)" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11298E10-21DD-4EBF-8BF9-EA571BEEC72E}" name="Table1" displayName="Table1" ref="A2:I127" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A2:I127" xr:uid="{11298E10-21DD-4EBF-8BF9-EA571BEEC72E}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{324771F9-822A-49B7-893D-1DA308D60F66}" name="Achievment" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{B22A3C33-D5FF-489D-81A0-0CD56EF167F6}" name="In-game description" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{3735BB57-B1D2-421D-9276-41B28AD37626}" name="Actual requirements (if different)" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{F9AD4A86-89AB-4252-BDC8-8698B593B077}" name="#" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{36B12DC4-1FAB-47F0-B495-DEEF3597AFFC}" name="Category" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{8DA34B88-F916-4B29-AA18-6228488B3C65}" name="Object" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{132DC9C0-CA6E-4B12-886A-9AB9F8BB67DB}" name="Index" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{ED2AFE63-C022-4969-A969-B12DDDC6F848}" name="Achievement (English Title)" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{A2DD8B78-9D4B-4932-958E-405ADE709BD5}" name="Column1" dataDxfId="1">
+      <calculatedColumnFormula>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54FDD79E-9496-444E-BAAB-2BDD7213F39D}" name="Table2" displayName="Table2" ref="A2:H112" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54FDD79E-9496-444E-BAAB-2BDD7213F39D}" name="Table2" displayName="Table2" ref="A2:H112" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A2:H112" xr:uid="{54FDD79E-9496-444E-BAAB-2BDD7213F39D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E112">
     <sortCondition ref="D2:D112"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{28B57E88-78E1-4471-B423-47178E900D39}" name="Advancement" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{3330A286-8064-4F71-8D6D-082AF5351B16}" name="In-game description" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{C6C9DE83-41CB-42D6-BAFA-5804D4D2C45F}" name="Actual requirements (if different)" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{27AB76C4-3016-4553-A87A-9C1F759A0798}" name="#" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{FF11131C-C5A2-4438-95D7-DCC625EAB401}" name="Column1" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{82ED0A77-34F2-4BBE-A373-52F72CBA1F8D}" name="Object" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{DB75B182-1053-43D2-9CB9-47C7FFF3DEDE}" name="Index" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{81839B7A-887C-4908-8072-601F3ED76542}" name="Advancement (English Title)" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{28B57E88-78E1-4471-B423-47178E900D39}" name="Advancement" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{3330A286-8064-4F71-8D6D-082AF5351B16}" name="In-game description" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{C6C9DE83-41CB-42D6-BAFA-5804D4D2C45F}" name="Actual requirements (if different)" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{27AB76C4-3016-4553-A87A-9C1F759A0798}" name="#" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{FF11131C-C5A2-4438-95D7-DCC625EAB401}" name="Column1" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{82ED0A77-34F2-4BBE-A373-52F72CBA1F8D}" name="Object" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{DB75B182-1053-43D2-9CB9-47C7FFF3DEDE}" name="Index" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{81839B7A-887C-4908-8072-601F3ED76542}" name="Advancement (English Title)" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2368,10 +2385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H127"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="D14" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2379,11 +2396,13 @@
     <col min="1" max="1" width="35.5703125" style="2" customWidth="1"/>
     <col min="2" max="3" width="50.5703125" style="1"/>
     <col min="4" max="4" width="5.5703125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="50.5703125" style="1"/>
+    <col min="5" max="6" width="50.5703125" style="1"/>
+    <col min="7" max="7" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="50.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>636</v>
       </c>
@@ -2408,8 +2427,11 @@
       <c r="H2" s="1" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>249</v>
       </c>
@@ -2434,8 +2456,12 @@
       <c r="H3" s="1" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>102</v>
       </c>
@@ -2460,8 +2486,12 @@
       <c r="H4" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I4" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -2486,8 +2516,12 @@
       <c r="H5" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I5" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>288</v>
       </c>
@@ -2512,8 +2546,12 @@
       <c r="H6" s="1" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>109</v>
       </c>
@@ -2538,8 +2576,12 @@
       <c r="H7" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -2564,8 +2606,12 @@
       <c r="H8" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>285</v>
       </c>
@@ -2590,8 +2636,12 @@
       <c r="H9" s="1" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -2616,8 +2666,12 @@
       <c r="H10" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>278</v>
       </c>
@@ -2642,8 +2696,12 @@
       <c r="H11" s="1" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>99</v>
       </c>
@@ -2668,8 +2726,12 @@
       <c r="H12" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I12" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
@@ -2694,8 +2756,12 @@
       <c r="H13" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I13" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>170</v>
       </c>
@@ -2720,8 +2786,12 @@
       <c r="H14" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>291</v>
       </c>
@@ -2746,8 +2816,12 @@
       <c r="H15" s="1" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I15" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>164</v>
       </c>
@@ -2772,8 +2846,12 @@
       <c r="H16" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
@@ -2798,8 +2876,12 @@
       <c r="H17" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I17" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>313</v>
       </c>
@@ -2824,8 +2906,12 @@
       <c r="H18" s="1" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I18" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>228</v>
       </c>
@@ -2850,8 +2936,12 @@
       <c r="H19" s="1" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>68</v>
       </c>
@@ -2876,8 +2966,12 @@
       <c r="H20" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>125</v>
       </c>
@@ -2902,8 +2996,12 @@
       <c r="H21" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Nether11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>209</v>
       </c>
@@ -2928,8 +3026,12 @@
       <c r="H22" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Nether12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>122</v>
       </c>
@@ -2954,8 +3056,12 @@
       <c r="H23" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I23" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Nether13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>149</v>
       </c>
@@ -2980,8 +3086,12 @@
       <c r="H24" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I24" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Nether14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>268</v>
       </c>
@@ -3006,8 +3116,12 @@
       <c r="H25" s="1" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>The_End11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>265</v>
       </c>
@@ -3032,8 +3146,12 @@
       <c r="H26" s="1" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I26" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>The_End12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>83</v>
       </c>
@@ -3058,8 +3176,12 @@
       <c r="H27" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I27" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>180</v>
       </c>
@@ -3084,8 +3206,12 @@
       <c r="H28" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I28" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>144</v>
       </c>
@@ -3110,8 +3236,12 @@
       <c r="H29" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I29" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
@@ -3136,8 +3266,12 @@
       <c r="H30" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I30" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>257</v>
       </c>
@@ -3157,13 +3291,17 @@
         <v>628</v>
       </c>
       <c r="G31" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I31" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Nether15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>260</v>
       </c>
@@ -3183,13 +3321,17 @@
         <v>628</v>
       </c>
       <c r="G32" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I32" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Nether16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>254</v>
       </c>
@@ -3209,13 +3351,17 @@
         <v>628</v>
       </c>
       <c r="G33" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Nether17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>206</v>
       </c>
@@ -3235,13 +3381,17 @@
         <v>625</v>
       </c>
       <c r="G34" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I34" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>65</v>
       </c>
@@ -3266,8 +3416,12 @@
       <c r="H35" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>183</v>
       </c>
@@ -3292,8 +3446,12 @@
       <c r="H36" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I36" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>161</v>
       </c>
@@ -3318,8 +3476,12 @@
       <c r="H37" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>73</v>
       </c>
@@ -3344,8 +3506,12 @@
       <c r="H38" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I38" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>139</v>
       </c>
@@ -3365,13 +3531,17 @@
         <v>625</v>
       </c>
       <c r="G39" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>194</v>
       </c>
@@ -3391,13 +3561,17 @@
         <v>625</v>
       </c>
       <c r="G40" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I40" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>186</v>
       </c>
@@ -3422,8 +3596,12 @@
       <c r="H41" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I41" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>273</v>
       </c>
@@ -3448,8 +3626,12 @@
       <c r="H42" s="1" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>196</v>
       </c>
@@ -3474,8 +3656,12 @@
       <c r="H43" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>135</v>
       </c>
@@ -3500,8 +3686,12 @@
       <c r="H44" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I44" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>128</v>
       </c>
@@ -3526,8 +3716,12 @@
       <c r="H45" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>107</v>
       </c>
@@ -3547,13 +3741,17 @@
         <v>625</v>
       </c>
       <c r="G46" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I46" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>200</v>
       </c>
@@ -3573,13 +3771,17 @@
         <v>625</v>
       </c>
       <c r="G47" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>241</v>
       </c>
@@ -3604,8 +3806,12 @@
       <c r="H48" s="1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I48" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
@@ -3630,8 +3836,12 @@
       <c r="H49" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I49" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>203</v>
       </c>
@@ -3656,8 +3866,12 @@
       <c r="H50" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>34</v>
       </c>
@@ -3677,13 +3891,17 @@
         <v>625</v>
       </c>
       <c r="G51" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>131</v>
       </c>
@@ -3708,8 +3926,12 @@
       <c r="H52" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I52" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>325</v>
       </c>
@@ -3729,13 +3951,17 @@
         <v>625</v>
       </c>
       <c r="G53" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>147</v>
       </c>
@@ -3755,13 +3981,17 @@
         <v>625</v>
       </c>
       <c r="G54" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry113</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>14</v>
       </c>
@@ -3786,8 +4016,12 @@
       <c r="H55" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I55" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>281</v>
       </c>
@@ -3812,8 +4046,12 @@
       <c r="H56" s="1" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>299</v>
       </c>
@@ -3838,8 +4076,12 @@
       <c r="H57" s="1" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>41</v>
       </c>
@@ -3864,8 +4106,12 @@
       <c r="H58" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I58" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure113</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>152</v>
       </c>
@@ -3890,8 +4136,12 @@
       <c r="H59" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I59" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>94</v>
       </c>
@@ -3916,8 +4166,12 @@
       <c r="H60" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I60" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>220</v>
       </c>
@@ -3942,8 +4196,12 @@
       <c r="H61" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I61" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story124</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>251</v>
       </c>
@@ -3968,8 +4226,12 @@
       <c r="H62" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I62" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure114</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>120</v>
       </c>
@@ -3989,13 +4251,17 @@
         <v>624</v>
       </c>
       <c r="G63" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>212</v>
       </c>
@@ -4015,13 +4281,17 @@
         <v>625</v>
       </c>
       <c r="G64" s="1">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry114</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>16</v>
       </c>
@@ -4041,13 +4311,17 @@
         <v>625</v>
       </c>
       <c r="G65" s="1">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I65" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry115</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>91</v>
       </c>
@@ -4072,8 +4346,12 @@
       <c r="H66" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure115</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>198</v>
       </c>
@@ -4093,13 +4371,17 @@
         <v>625</v>
       </c>
       <c r="G67" s="1">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry116</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>263</v>
       </c>
@@ -4124,8 +4406,12 @@
       <c r="H68" s="1" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure116</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>78</v>
       </c>
@@ -4145,13 +4431,17 @@
         <v>624</v>
       </c>
       <c r="G69" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>245</v>
       </c>
@@ -4171,13 +4461,17 @@
         <v>624</v>
       </c>
       <c r="G70" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story127</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>322</v>
       </c>
@@ -4202,8 +4496,12 @@
       <c r="H71" s="1" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I71" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>The_End13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>23</v>
       </c>
@@ -4223,13 +4521,17 @@
         <v>628</v>
       </c>
       <c r="G72" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Nether18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>271</v>
       </c>
@@ -4254,8 +4556,12 @@
       <c r="H73" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>The_End14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>105</v>
       </c>
@@ -4280,8 +4586,12 @@
       <c r="H74" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I74" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>The_End15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>247</v>
       </c>
@@ -4306,8 +4616,12 @@
       <c r="H75" s="1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I75" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>The_End16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>301</v>
       </c>
@@ -4332,8 +4646,12 @@
       <c r="H76" s="1" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure117</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>178</v>
       </c>
@@ -4358,8 +4676,12 @@
       <c r="H77" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I77" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>The_End17</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>50</v>
       </c>
@@ -4384,8 +4706,12 @@
       <c r="H78" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure118</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>86</v>
       </c>
@@ -4410,8 +4736,12 @@
       <c r="H79" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I79" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure119</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>142</v>
       </c>
@@ -4436,8 +4766,12 @@
       <c r="H80" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure120</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>231</v>
       </c>
@@ -4457,13 +4791,17 @@
         <v>625</v>
       </c>
       <c r="G81" s="1">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry117</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>18</v>
       </c>
@@ -4488,8 +4826,12 @@
       <c r="H82" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I82" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure121</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>214</v>
       </c>
@@ -4514,8 +4856,12 @@
       <c r="H83" s="1" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I83" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure122</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>45</v>
       </c>
@@ -4540,8 +4886,12 @@
       <c r="H84" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure123</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>8</v>
       </c>
@@ -4566,8 +4916,12 @@
       <c r="H85" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure124</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>115</v>
       </c>
@@ -4587,13 +4941,17 @@
         <v>625</v>
       </c>
       <c r="G86" s="1">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry118</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>158</v>
       </c>
@@ -4618,8 +4976,12 @@
       <c r="H87" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure125</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>217</v>
       </c>
@@ -4639,13 +5001,17 @@
         <v>627</v>
       </c>
       <c r="G88" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I88" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure126</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>11</v>
       </c>
@@ -4665,13 +5031,17 @@
         <v>624</v>
       </c>
       <c r="G89" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I89" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story128</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>75</v>
       </c>
@@ -4691,13 +5061,17 @@
         <v>627</v>
       </c>
       <c r="G90" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I90" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure127</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>173</v>
       </c>
@@ -4717,13 +5091,17 @@
         <v>624</v>
       </c>
       <c r="G91" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I91" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story129</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>80</v>
       </c>
@@ -4743,13 +5121,17 @@
         <v>627</v>
       </c>
       <c r="G92" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I92" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure128</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>167</v>
       </c>
@@ -4769,13 +5151,17 @@
         <v>624</v>
       </c>
       <c r="G93" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story130</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>294</v>
       </c>
@@ -4795,13 +5181,17 @@
         <v>624</v>
       </c>
       <c r="G94" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story131</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>316</v>
       </c>
@@ -4821,13 +5211,17 @@
         <v>625</v>
       </c>
       <c r="G95" s="1">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry119</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>328</v>
       </c>
@@ -4847,13 +5241,17 @@
         <v>625</v>
       </c>
       <c r="G96" s="1">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry120</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>96</v>
       </c>
@@ -4873,13 +5271,17 @@
         <v>624</v>
       </c>
       <c r="G97" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I97" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story132</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>191</v>
       </c>
@@ -4899,13 +5301,17 @@
         <v>625</v>
       </c>
       <c r="G98" s="1">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry121</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>137</v>
       </c>
@@ -4925,13 +5331,17 @@
         <v>627</v>
       </c>
       <c r="G99" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I99" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure129</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>38</v>
       </c>
@@ -4948,16 +5358,20 @@
         <v>623</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>624</v>
+        <v>631</v>
       </c>
       <c r="G100" s="1">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I100" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story21</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>71</v>
       </c>
@@ -4977,13 +5391,17 @@
         <v>631</v>
       </c>
       <c r="G101" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>307</v>
       </c>
@@ -5003,13 +5421,17 @@
         <v>627</v>
       </c>
       <c r="G102" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I102" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure130</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>236</v>
       </c>
@@ -5029,13 +5451,17 @@
         <v>631</v>
       </c>
       <c r="G103" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I103" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story23</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>118</v>
       </c>
@@ -5055,13 +5481,17 @@
         <v>627</v>
       </c>
       <c r="G104" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H104" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I104" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure131</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>155</v>
       </c>
@@ -5081,13 +5511,17 @@
         <v>631</v>
       </c>
       <c r="G105" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H105" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I105" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story24</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>283</v>
       </c>
@@ -5107,13 +5541,17 @@
         <v>631</v>
       </c>
       <c r="G106" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I106" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story25</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>26</v>
       </c>
@@ -5133,13 +5571,17 @@
         <v>625</v>
       </c>
       <c r="G107" s="1">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I107" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry122</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>297</v>
       </c>
@@ -5159,13 +5601,17 @@
         <v>625</v>
       </c>
       <c r="G108" s="1">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I108" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry123</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>243</v>
       </c>
@@ -5185,13 +5631,17 @@
         <v>631</v>
       </c>
       <c r="G109" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H109" s="1" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I109" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story26</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>36</v>
       </c>
@@ -5211,13 +5661,17 @@
         <v>631</v>
       </c>
       <c r="G110" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H110" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I110" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story27</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>56</v>
       </c>
@@ -5237,13 +5691,17 @@
         <v>628</v>
       </c>
       <c r="G111" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H111" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I111" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Nether19</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>175</v>
       </c>
@@ -5263,13 +5721,17 @@
         <v>628</v>
       </c>
       <c r="G112" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H112" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I112" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Nether110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>112</v>
       </c>
@@ -5289,13 +5751,17 @@
         <v>628</v>
       </c>
       <c r="G113" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H113" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I113" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Nether111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>310</v>
       </c>
@@ -5315,13 +5781,17 @@
         <v>627</v>
       </c>
       <c r="G114" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H114" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I114" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure132</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>304</v>
       </c>
@@ -5341,13 +5811,17 @@
         <v>631</v>
       </c>
       <c r="G115" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I115" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story28</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>275</v>
       </c>
@@ -5367,13 +5841,17 @@
         <v>625</v>
       </c>
       <c r="G116" s="1">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H116" s="1" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I116" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry124</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>48</v>
       </c>
@@ -5393,13 +5871,17 @@
         <v>631</v>
       </c>
       <c r="G117" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I117" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story29</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>238</v>
       </c>
@@ -5419,13 +5901,17 @@
         <v>631</v>
       </c>
       <c r="G118" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H118" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I118" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story210</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>233</v>
       </c>
@@ -5445,13 +5931,17 @@
         <v>631</v>
       </c>
       <c r="G119" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H119" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I119" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story211</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>88</v>
       </c>
@@ -5471,13 +5961,17 @@
         <v>628</v>
       </c>
       <c r="G120" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H120" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I120" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Nether112</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>133</v>
       </c>
@@ -5497,13 +5991,17 @@
         <v>631</v>
       </c>
       <c r="G121" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H121" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I121" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story212</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>31</v>
       </c>
@@ -5523,13 +6021,17 @@
         <v>625</v>
       </c>
       <c r="G122" s="1">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H122" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I122" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry125</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>319</v>
       </c>
@@ -5549,13 +6051,17 @@
         <v>628</v>
       </c>
       <c r="G123" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H123" s="1" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I123" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Nether113</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>225</v>
       </c>
@@ -5575,13 +6081,17 @@
         <v>631</v>
       </c>
       <c r="G124" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H124" s="1" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I124" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story213</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>189</v>
       </c>
@@ -5601,13 +6111,17 @@
         <v>631</v>
       </c>
       <c r="G125" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H125" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I125" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story214</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>43</v>
       </c>
@@ -5627,13 +6141,17 @@
         <v>631</v>
       </c>
       <c r="G126" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H126" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I126" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story215</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>223</v>
       </c>
@@ -5653,14 +6171,21 @@
         <v>631</v>
       </c>
       <c r="G127" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H127" s="1" t="s">
         <v>223</v>
       </c>
+      <c r="I127" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Object]],Table1[[#This Row],[Index]])</f>
+        <v>Story216</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -5672,8 +6197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771D2FCF-03EA-4C2E-BCB7-15D3321DB186}">
   <dimension ref="A2:H112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6774,7 +7299,6 @@
         <v>630</v>
       </c>
       <c r="G43" s="1">
-        <f>1</f>
         <v>1</v>
       </c>
       <c r="H43" s="1" t="s">
@@ -6905,8 +7429,7 @@
         <v>630</v>
       </c>
       <c r="G48" s="1">
-        <f>1</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>322</v>
@@ -6932,7 +7455,7 @@
         <v>630</v>
       </c>
       <c r="G49" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>446</v>
@@ -6958,7 +7481,7 @@
         <v>630</v>
       </c>
       <c r="G50" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>449</v>
@@ -6984,7 +7507,7 @@
         <v>630</v>
       </c>
       <c r="G51" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>105</v>
@@ -7010,7 +7533,6 @@
         <v>627</v>
       </c>
       <c r="G52" s="1">
-        <f>1</f>
         <v>1</v>
       </c>
       <c r="H52" s="1" t="s">

</xml_diff>